<commit_message>
add data and legend
</commit_message>
<xml_diff>
--- a/doc/Workbook1_buda.xlsx
+++ b/doc/Workbook1_buda.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="0" windowWidth="25600" windowHeight="16660" tabRatio="500"/>
+    <workbookView xWindow="1620" yWindow="0" windowWidth="25560" windowHeight="9500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -154,7 +154,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -167,6 +167,22 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,8 +202,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -196,7 +216,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -526,15 +550,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:O14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -560,7 +584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" s="2">
         <v>19.010090999999999</v>
       </c>
@@ -606,8 +630,12 @@
       <c r="O2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2" t="str">
+        <f>I2&amp;C2&amp;J2&amp;H2&amp;K2&amp;A2&amp;L2&amp;B2&amp;M2&amp;A2&amp;N2&amp;B2&amp;O2</f>
+        <v>{"type":"Feature","properties":{"Code":"BUD31",Name":"official, Budatétény","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,010091,"Lat":47,406033, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,010091,47,406033]]},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>19.041043999999999</v>
       </c>
@@ -653,8 +681,12 @@
       <c r="O3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3" t="str">
+        <f t="shared" ref="P3:P14" si="0">I3&amp;C3&amp;J3&amp;H3&amp;K3&amp;A3&amp;L3&amp;B3&amp;M3&amp;A3&amp;N3&amp;B3&amp;O3</f>
+        <v>{"type":"Feature","properties":{"Code":"BUD32",Name":"official, Kosztolányi D. tér","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,041044,"Lat":47,474894, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,041044,47,474894]]},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>19.040355999999999</v>
       </c>
@@ -700,8 +732,12 @@
       <c r="O4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4" t="str">
+        <f t="shared" si="0"/>
+        <v>{"type":"Feature","properties":{"Code":"BUD33",Name":"official, Clar Adam tér","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,040356,"Lat":47,497885, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,040356,47,497885]]},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>19.027743000000001</v>
       </c>
@@ -747,8 +783,12 @@
       <c r="O5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5" t="str">
+        <f t="shared" si="0"/>
+        <v>{"type":"Feature","properties":{"Code":"BUD34",Name":"official, Széna tér","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,027743,"Lat":47,508683, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,027743,47,508683]]},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>19.052054999999999</v>
       </c>
@@ -794,8 +834,12 @@
       <c r="O6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6" t="str">
+        <f t="shared" si="0"/>
+        <v>{"type":"Feature","properties":{"Code":"BUD35",Name":"official, Erzsébet tér","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,052055,"Lat":47,498929, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,052055,47,498929]]},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>19.087776999999999</v>
       </c>
@@ -841,8 +885,12 @@
       <c r="O7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7" t="str">
+        <f t="shared" si="0"/>
+        <v>{"type":"Feature","properties":{"Code":"BUD36",Name":"official, Teleki tér","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,087777,"Lat":47,492115, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,087777,47,492115]]},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>19.157288999999999</v>
       </c>
@@ -888,8 +936,12 @@
       <c r="O8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8" t="str">
+        <f t="shared" si="0"/>
+        <v>{"type":"Feature","properties":{"Code":"BUD37",Name":"official, Gergely utca","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,157289,"Lat":47,466992, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,157289,47,466992]]},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>19.091177999999999</v>
       </c>
@@ -935,8 +987,12 @@
       <c r="O9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9" t="str">
+        <f t="shared" si="0"/>
+        <v>{"type":"Feature","properties":{"Code":"BUD38",Name":"official, Budapest, Csepel","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,091178,"Lat":47,404439, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,091178,47,404439]]},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>19.069613</v>
       </c>
@@ -982,8 +1038,12 @@
       <c r="O10" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10" t="str">
+        <f t="shared" si="0"/>
+        <v>{"type":"Feature","properties":{"Code":"BUD39",Name":"official, Budapest, Honvéd","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,069613,"Lat":47,522873, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,069613,47,522873]]},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>19.144145000000002</v>
       </c>
@@ -1029,8 +1089,12 @@
       <c r="O11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11" t="str">
+        <f t="shared" si="0"/>
+        <v>{"type":"Feature","properties":{"Code":"BUD40",Name":"officiíal, Kőrakás park","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,144145,"Lat":47,544335, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,144145,47,544335]]},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>19.114628</v>
       </c>
@@ -1076,8 +1140,12 @@
       <c r="O12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12" t="str">
+        <f t="shared" si="0"/>
+        <v>{"type":"Feature","properties":{"Code":"BUD41",Name":"official, Káposztásmegyer","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,114628,"Lat":47,581917, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,114628,47,581917]]},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>18.960754999999999</v>
       </c>
@@ -1123,8 +1191,12 @@
       <c r="O13" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13" t="str">
+        <f t="shared" si="0"/>
+        <v>{"type":"Feature","properties":{"Code":"BUD42",Name":"official, Pesthidegkút","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":18,960755,"Lat":47,561682, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[18,960755,47,561682]]},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>19.181107999999998</v>
       </c>
@@ -1170,9 +1242,14 @@
       <c r="O14" t="s">
         <v>42</v>
       </c>
+      <c r="P14" t="str">
+        <f t="shared" si="0"/>
+        <v>{"type":"Feature","properties":{"Code":"BUD43",Name":"official, Gilice tér","CountryCode":"HU","Country":"Hungary","Location":"Budapest","Lon":19,181108,"Lat":47,430192, "AreaClassification":"Urban","StationClassification":"Traffic"},"geometry": {"type": "MultiPoint","coordinates":[[19,181108,47,430192]]},</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>